<commit_message>
Query 1: added % in query directly
</commit_message>
<xml_diff>
--- a/query1-results.xlsx
+++ b/query1-results.xlsx
@@ -441,17 +441,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>on_time_flights</t>
+          <t>on_time_percentage</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>late_flights</t>
+          <t>late_percentage</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>cancelled_flights</t>
+          <t>cancelled_percentage</t>
         </is>
       </c>
     </row>
@@ -465,13 +465,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>624</v>
+        <v>93.41</v>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>2.99</v>
       </c>
       <c r="E2" t="n">
-        <v>24</v>
+        <v>3.59</v>
       </c>
     </row>
     <row r="3">
@@ -484,13 +484,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>982</v>
+        <v>96.94</v>
       </c>
       <c r="D3" t="n">
-        <v>28</v>
+        <v>2.76</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4">
@@ -503,13 +503,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>646</v>
+        <v>94.58</v>
       </c>
       <c r="D4" t="n">
-        <v>22</v>
+        <v>3.22</v>
       </c>
       <c r="E4" t="n">
-        <v>15</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="5">
@@ -522,13 +522,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>612</v>
+        <v>95.77</v>
       </c>
       <c r="D5" t="n">
-        <v>21</v>
+        <v>3.29</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>307</v>
+        <v>96.54000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>10</v>
+        <v>3.14</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="7">
@@ -560,13 +560,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4674</v>
+        <v>94.87</v>
       </c>
       <c r="D7" t="n">
-        <v>138</v>
+        <v>2.8</v>
       </c>
       <c r="E7" t="n">
-        <v>115</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="8">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4570</v>
+        <v>93.27</v>
       </c>
       <c r="D8" t="n">
-        <v>149</v>
+        <v>3.04</v>
       </c>
       <c r="E8" t="n">
-        <v>181</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="9">
@@ -598,13 +598,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4292</v>
+        <v>95.56999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>130</v>
+        <v>2.89</v>
       </c>
       <c r="E9" t="n">
-        <v>69</v>
+        <v>1.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>